<commit_message>
Kleine Fehlerbehebungen und Code lässt sich ausführen
</commit_message>
<xml_diff>
--- a/data/Leistungskurve_data.xlsx
+++ b/data/Leistungskurve_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/janik/PycharmProjects/EWM-Grupp1/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11EF736C-D783-A243-AA75-BEF90C3608E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C407587-84E6-2641-8DD8-2F3134C5FA04}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="660" windowWidth="13200" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44240" yWindow="7100" windowWidth="13200" windowHeight="14220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wind_vs_Power" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
     <t>Windgeschwindigkeit (mph)</t>
   </si>
   <si>
-    <t>Leistung</t>
+    <t>Leistung (W)</t>
   </si>
 </sst>
 </file>
@@ -396,7 +396,7 @@
   <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>